<commit_message>
Fixed some labels in Feeds_Speeds_Vs_Material.xlsx
</commit_message>
<xml_diff>
--- a/Feeds_Speeds_Vs_Material.xlsx
+++ b/Feeds_Speeds_Vs_Material.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fende\Documents\CAD\CNC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fende\SRC\Axiom_i2r_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682BF76B-1F33-4ACC-96B7-E7C0605BD2A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3D2843-E057-433E-BFA4-E7226D2731FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2Flute" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="338">
   <si>
     <t>Type</t>
   </si>
@@ -877,178 +877,175 @@
 (RPM)</t>
   </si>
   <si>
-    <t>12.43mm3</t>
-  </si>
-  <si>
-    <t>0.76in3</t>
-  </si>
-  <si>
-    <t>10.66mm3</t>
-  </si>
-  <si>
-    <t>0.65in3</t>
-  </si>
-  <si>
-    <t>14.21mm3</t>
-  </si>
-  <si>
-    <t>0.87in3</t>
-  </si>
-  <si>
-    <t>27.33mm3</t>
-  </si>
-  <si>
-    <t>1.67in3</t>
-  </si>
-  <si>
-    <t>12.02mm3</t>
-  </si>
-  <si>
-    <t>0.73in3</t>
-  </si>
-  <si>
-    <t>16.39mm3</t>
-  </si>
-  <si>
-    <t>1in3</t>
-  </si>
-  <si>
-    <t>6.15mm3</t>
-  </si>
-  <si>
-    <t>0.38in3</t>
-  </si>
-  <si>
-    <t>19.67mm3</t>
-  </si>
-  <si>
-    <t>1.2in3</t>
-  </si>
-  <si>
-    <t>8.6mm3</t>
-  </si>
-  <si>
-    <t>0.53in3</t>
-  </si>
-  <si>
-    <t>3.28mm3</t>
-  </si>
-  <si>
-    <t>0.2in3</t>
-  </si>
-  <si>
-    <t>20.49mm3</t>
-  </si>
-  <si>
-    <t>1.25in3</t>
-  </si>
-  <si>
-    <t>35.52mm3</t>
-  </si>
-  <si>
-    <t>2.17in3</t>
-  </si>
-  <si>
-    <t>14.76mm3</t>
-  </si>
-  <si>
-    <t>0.9in3</t>
-  </si>
-  <si>
-    <t>17.76mm3</t>
-  </si>
-  <si>
-    <t>1.08in3</t>
-  </si>
-  <si>
-    <t>7.38mm3</t>
-  </si>
-  <si>
-    <t>0.45in3</t>
-  </si>
-  <si>
-    <t>36.89mm3</t>
-  </si>
-  <si>
-    <t>2.25in3</t>
-  </si>
-  <si>
-    <t>2.46mm3</t>
-  </si>
-  <si>
-    <t>0.15in3</t>
-  </si>
-  <si>
-    <t>1.37mm3</t>
-  </si>
-  <si>
-    <t>0.08in3</t>
-  </si>
-  <si>
-    <t>8.88mm3</t>
-  </si>
-  <si>
-    <t>0.54in3</t>
-  </si>
-  <si>
-    <t>4.37mm3</t>
-  </si>
-  <si>
-    <t>0.27in3</t>
-  </si>
-  <si>
-    <t>0.66mm3</t>
-  </si>
-  <si>
-    <t>0.04in3</t>
-  </si>
-  <si>
-    <t>39.07mm3</t>
-  </si>
-  <si>
-    <t>2.38in3</t>
-  </si>
-  <si>
-    <t>81.98mm3</t>
-  </si>
-  <si>
-    <t>5in3</t>
-  </si>
-  <si>
-    <t>68.31mm3</t>
-  </si>
-  <si>
-    <t>4.17in3</t>
-  </si>
-  <si>
-    <t>65.58mm3</t>
-  </si>
-  <si>
-    <t>4in3</t>
-  </si>
-  <si>
-    <t>49.19mm3</t>
-  </si>
-  <si>
-    <t>3in3</t>
-  </si>
-  <si>
-    <t>5.47mm3</t>
-  </si>
-  <si>
-    <t>0.33in3</t>
-  </si>
-  <si>
-    <t>10.93mm3</t>
-  </si>
-  <si>
-    <t>0.67in3</t>
-  </si>
-  <si>
-    <t>0mm3</t>
-  </si>
-  <si>
-    <t>0in3</t>
+    <t>Endmill</t>
+  </si>
+  <si>
+    <t>12.43mm3/min</t>
+  </si>
+  <si>
+    <t>0.76in3/min</t>
+  </si>
+  <si>
+    <t>10.66mm3/min</t>
+  </si>
+  <si>
+    <t>0.65in3/min</t>
+  </si>
+  <si>
+    <t>14.21mm3/min</t>
+  </si>
+  <si>
+    <t>0.87in3/min</t>
+  </si>
+  <si>
+    <t>27.33mm3/min</t>
+  </si>
+  <si>
+    <t>1.67in3/min</t>
+  </si>
+  <si>
+    <t>12.02mm3/min</t>
+  </si>
+  <si>
+    <t>0.73in3/min</t>
+  </si>
+  <si>
+    <t>16.39mm3/min</t>
+  </si>
+  <si>
+    <t>1in3/min</t>
+  </si>
+  <si>
+    <t>6.15mm3/min</t>
+  </si>
+  <si>
+    <t>0.38in3/min</t>
+  </si>
+  <si>
+    <t>19.67mm3/min</t>
+  </si>
+  <si>
+    <t>1.2in3/min</t>
+  </si>
+  <si>
+    <t>8.6mm3/min</t>
+  </si>
+  <si>
+    <t>0.53in3/min</t>
+  </si>
+  <si>
+    <t>3.28mm3/min</t>
+  </si>
+  <si>
+    <t>0.2in3/min</t>
+  </si>
+  <si>
+    <t>20.49mm3/min</t>
+  </si>
+  <si>
+    <t>1.25in3/min</t>
+  </si>
+  <si>
+    <t>35.52mm3/min</t>
+  </si>
+  <si>
+    <t>2.17in3/min</t>
+  </si>
+  <si>
+    <t>14.76mm3/min</t>
+  </si>
+  <si>
+    <t>0.9in3/min</t>
+  </si>
+  <si>
+    <t>17.76mm3/min</t>
+  </si>
+  <si>
+    <t>1.08in3/min</t>
+  </si>
+  <si>
+    <t>7.38mm3/min</t>
+  </si>
+  <si>
+    <t>0.45in3/min</t>
+  </si>
+  <si>
+    <t>36.89mm3/min</t>
+  </si>
+  <si>
+    <t>2.25in3/min</t>
+  </si>
+  <si>
+    <t>2.46mm3/min</t>
+  </si>
+  <si>
+    <t>0.15in3/min</t>
+  </si>
+  <si>
+    <t>1.37mm3/min</t>
+  </si>
+  <si>
+    <t>0.08in3/min</t>
+  </si>
+  <si>
+    <t>8.88mm3/min</t>
+  </si>
+  <si>
+    <t>0.54in3/min</t>
+  </si>
+  <si>
+    <t>4.37mm3/min</t>
+  </si>
+  <si>
+    <t>0.27in3/min</t>
+  </si>
+  <si>
+    <t>0.66mm3/min</t>
+  </si>
+  <si>
+    <t>0.04in3/min</t>
+  </si>
+  <si>
+    <t>39.07mm3/min</t>
+  </si>
+  <si>
+    <t>2.38in3/min</t>
+  </si>
+  <si>
+    <t>81.98mm3/min</t>
+  </si>
+  <si>
+    <t>5in3/min</t>
+  </si>
+  <si>
+    <t>68.31mm3/min</t>
+  </si>
+  <si>
+    <t>4.17in3/min</t>
+  </si>
+  <si>
+    <t>65.58mm3/min</t>
+  </si>
+  <si>
+    <t>4in3/min</t>
+  </si>
+  <si>
+    <t>49.19mm3/min</t>
+  </si>
+  <si>
+    <t>3in3/min</t>
+  </si>
+  <si>
+    <t>5.47mm3/min</t>
+  </si>
+  <si>
+    <t>0.33in3/min</t>
+  </si>
+  <si>
+    <t>10.93mm3/min</t>
+  </si>
+  <si>
+    <t>0.67in3/min</t>
   </si>
 </sst>
 </file>
@@ -1538,23 +1535,23 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.21875" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="37.109375" style="14"/>
   </cols>
   <sheetData>
@@ -1566,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1619,7 +1616,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1643,7 +1640,7 @@
         <v>217</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1675,7 +1672,7 @@
         <v>218</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1699,7 +1696,7 @@
         <v>219</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1731,7 +1728,7 @@
         <v>220</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1755,7 +1752,7 @@
         <v>221</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1787,7 +1784,7 @@
         <v>222</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1811,7 +1808,7 @@
         <v>223</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1843,7 +1840,7 @@
         <v>224</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1867,7 +1864,7 @@
         <v>225</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1899,7 +1896,7 @@
         <v>226</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1923,7 +1920,7 @@
         <v>227</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1955,7 +1952,7 @@
         <v>226</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1979,7 +1976,7 @@
         <v>227</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2011,7 +2008,7 @@
         <v>226</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2035,7 +2032,7 @@
         <v>227</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2067,7 +2064,7 @@
         <v>224</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2091,7 +2088,7 @@
         <v>225</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2123,7 +2120,7 @@
         <v>228</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2147,7 +2144,7 @@
         <v>229</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2179,7 +2176,7 @@
         <v>230</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2203,7 +2200,7 @@
         <v>231</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2235,7 +2232,7 @@
         <v>232</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2259,7 +2256,7 @@
         <v>233</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2291,7 +2288,7 @@
         <v>234</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2315,7 +2312,7 @@
         <v>235</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2347,7 +2344,7 @@
         <v>236</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2371,7 +2368,7 @@
         <v>237</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -2403,7 +2400,7 @@
         <v>238</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2427,7 +2424,7 @@
         <v>239</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2459,7 +2456,7 @@
         <v>240</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -2483,7 +2480,7 @@
         <v>241</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -2515,7 +2512,7 @@
         <v>242</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -2539,7 +2536,7 @@
         <v>243</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -2571,7 +2568,7 @@
         <v>244</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -2595,7 +2592,7 @@
         <v>245</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2627,7 +2624,7 @@
         <v>246</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -2651,7 +2648,7 @@
         <v>247</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -2683,7 +2680,7 @@
         <v>224</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2707,7 +2704,7 @@
         <v>225</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -2739,7 +2736,7 @@
         <v>248</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -2763,7 +2760,7 @@
         <v>217</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -2795,7 +2792,7 @@
         <v>248</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -2819,7 +2816,7 @@
         <v>217</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2851,7 +2848,7 @@
         <v>244</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2875,7 +2872,7 @@
         <v>245</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -2907,7 +2904,7 @@
         <v>249</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -2931,7 +2928,7 @@
         <v>250</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -2963,7 +2960,7 @@
         <v>251</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -2987,7 +2984,7 @@
         <v>252</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3019,7 +3016,7 @@
         <v>253</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3043,7 +3040,7 @@
         <v>254</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -3075,7 +3072,7 @@
         <v>255</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -3099,7 +3096,7 @@
         <v>256</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -3131,7 +3128,7 @@
         <v>257</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -3155,7 +3152,7 @@
         <v>258</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -3187,7 +3184,7 @@
         <v>259</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -3211,7 +3208,7 @@
         <v>260</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -3243,7 +3240,7 @@
         <v>261</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -3267,7 +3264,7 @@
         <v>262</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -3299,7 +3296,7 @@
         <v>218</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -3323,7 +3320,7 @@
         <v>219</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -3355,7 +3352,7 @@
         <v>263</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -3379,7 +3376,7 @@
         <v>264</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -3411,7 +3408,7 @@
         <v>265</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -3435,7 +3432,7 @@
         <v>266</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -3467,7 +3464,7 @@
         <v>267</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -3491,7 +3488,7 @@
         <v>268</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -3523,7 +3520,7 @@
         <v>269</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -3547,7 +3544,7 @@
         <v>270</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -3579,7 +3576,7 @@
         <v>232</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -3603,7 +3600,7 @@
         <v>233</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -3635,7 +3632,7 @@
         <v>236</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -3659,50 +3656,29 @@
         <v>237</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F76" s="5"/>
-      <c r="J76" s="14" t="s">
-        <v>337</v>
-      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F77" s="5"/>
-      <c r="J77" s="14" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F78" s="5"/>
-      <c r="J78" s="14" t="s">
-        <v>337</v>
-      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F79" s="5"/>
-      <c r="J79" s="14" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F80" s="5"/>
-      <c r="J80" s="14" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="81" spans="6:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F81" s="5"/>
-      <c r="J81" s="14" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="82" spans="6:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F82" s="15"/>
-      <c r="J82" s="14" t="s">
-        <v>337</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3715,7 +3691,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>

</xml_diff>